<commit_message>
made some changes for admin panel
</commit_message>
<xml_diff>
--- a/uploads/excel-files/PG001/March/1741467716318-PG_Tenant_Data2.xlsx
+++ b/uploads/excel-files/PG001/March/1741467716318-PG_Tenant_Data2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\OneDrive\Desktop\RCMS\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\OneDrive\Desktop\RCMS\backend\uploads\excel-files\PG001\March\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8C6A18-9C1C-47B7-B0D2-A6A08A726474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542BE0B9-8A11-42F4-99E9-760BB15E1898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>pgId</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>301</t>
+  </si>
+  <si>
+    <t>PG005</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +462,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>

</xml_diff>